<commit_message>
my latest familt tree Excel file
</commit_message>
<xml_diff>
--- a/togod.xlsx
+++ b/togod.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Family Tree - All" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="363">
   <si>
     <t>Genealogy of Jesus according to Matthew</t>
   </si>
@@ -947,6 +947,171 @@
   </si>
   <si>
     <t>Spouse 2</t>
+  </si>
+  <si>
+    <t>Nancy Huddleston (1794-1865)</t>
+  </si>
+  <si>
+    <t>William Thomas (1793-1834)</t>
+  </si>
+  <si>
+    <t>Lawrence De CORNWALL b: Abt 1241 d: ####</t>
+  </si>
+  <si>
+    <t>Sybil DE CORNWALL b: #### d: ####</t>
+  </si>
+  <si>
+    <t>Lady Maud DE PENNINGTON b: #### d: ####</t>
+  </si>
+  <si>
+    <t>Joan UNKNOWN (Stapleton?) b: #### d: ####           OR</t>
+  </si>
+  <si>
+    <t>Anne Lady of C M Fenwicke b: 1403 d: ####              OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary FENWICK b: #### d: ####                                     OR </t>
+  </si>
+  <si>
+    <t>Joan Stapleton (?) b: #### d: ####</t>
+  </si>
+  <si>
+    <t>John HUDDLESTONE b: 1490 d: ####</t>
+  </si>
+  <si>
+    <t>Elizabeth SUTTON b: 1493 d: ####</t>
+  </si>
+  <si>
+    <t>Bridget COTTON b: 1530 d: ####</t>
+  </si>
+  <si>
+    <t>Dorthy BEACONSALL b: 1552 d: ####</t>
+  </si>
+  <si>
+    <t>Dorthy DORMER b: 1577 d: ####</t>
+  </si>
+  <si>
+    <t>Henry HUDDLESTON b: 1575 d: ####</t>
+  </si>
+  <si>
+    <t>Richard HUDDLESTON b: Abt 1660 d: ####</t>
+  </si>
+  <si>
+    <t>Mary BOSTOCK b: 1660 d: ####</t>
+  </si>
+  <si>
+    <t>Mary PATTERSON b: #### d: ####</t>
+  </si>
+  <si>
+    <t>Sarah GALLAWAY b: #### d: ####</t>
+  </si>
+  <si>
+    <t>Joan Or Jane De VALLETORT b: Abt 1213 d: ####</t>
+  </si>
+  <si>
+    <t>Thomas Holland (####-####)</t>
+  </si>
+  <si>
+    <t>George V (####-####)</t>
+  </si>
+  <si>
+    <t>Mary II (####-####)</t>
+  </si>
+  <si>
+    <t>George IV (####-####)</t>
+  </si>
+  <si>
+    <t>Edward Duke of Kent (####-####)</t>
+  </si>
+  <si>
+    <t>George III (####-####)</t>
+  </si>
+  <si>
+    <t>Frederick Prince of Wales (####-####)</t>
+  </si>
+  <si>
+    <t>George II (####-####)</t>
+  </si>
+  <si>
+    <t>George I (####-####)</t>
+  </si>
+  <si>
+    <t>Sophia (####-####)</t>
+  </si>
+  <si>
+    <t>Elizabeth Stewart (####-####)</t>
+  </si>
+  <si>
+    <t>James VI (####-####)</t>
+  </si>
+  <si>
+    <t>Mary Queen of Scots (####-####)</t>
+  </si>
+  <si>
+    <t>James V (####-####)</t>
+  </si>
+  <si>
+    <t>James III (####-####)</t>
+  </si>
+  <si>
+    <t>James II (####-####)</t>
+  </si>
+  <si>
+    <t>James I (####-####)</t>
+  </si>
+  <si>
+    <t>Robert III (####-####)</t>
+  </si>
+  <si>
+    <t>Robert II (####-####)</t>
+  </si>
+  <si>
+    <t>Marlory (####-####)</t>
+  </si>
+  <si>
+    <t>Robert the Bruce (####-####)</t>
+  </si>
+  <si>
+    <t>Robert (####-####)</t>
+  </si>
+  <si>
+    <t>Isabel (####-####)</t>
+  </si>
+  <si>
+    <t>David (####-####)</t>
+  </si>
+  <si>
+    <t>Henry (####-####)</t>
+  </si>
+  <si>
+    <t>Malcolm (####-####)</t>
+  </si>
+  <si>
+    <t>Duncan (####-####)</t>
+  </si>
+  <si>
+    <t>Beatrix (####-####)</t>
+  </si>
+  <si>
+    <t>Malcolm II (####-####)</t>
+  </si>
+  <si>
+    <t>Kenneth II (####-####)</t>
+  </si>
+  <si>
+    <t>Donald IV (####-####)</t>
+  </si>
+  <si>
+    <t>Constantine (####-####)</t>
+  </si>
+  <si>
+    <t>Kenneth the Alpin (####-####)</t>
+  </si>
+  <si>
+    <t>Marie Kenly (Antoine) Jonason (1972-####)</t>
+  </si>
+  <si>
+    <t>Gregory Alan (Johnson) Jonason (1973-####)</t>
   </si>
 </sst>
 </file>
@@ -1521,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="D179" sqref="D179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2580,7 +2745,7 @@
         <v>87</v>
       </c>
       <c r="D95" t="s">
-        <v>136</v>
+        <v>360</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2591,7 +2756,7 @@
         <v>86</v>
       </c>
       <c r="D96" t="s">
-        <v>135</v>
+        <v>359</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2602,7 +2767,7 @@
         <v>85</v>
       </c>
       <c r="D97" t="s">
-        <v>134</v>
+        <v>358</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2613,7 +2778,7 @@
         <v>84</v>
       </c>
       <c r="D98" t="s">
-        <v>129</v>
+        <v>353</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2624,7 +2789,7 @@
         <v>83</v>
       </c>
       <c r="D99" t="s">
-        <v>133</v>
+        <v>357</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2635,7 +2800,7 @@
         <v>82</v>
       </c>
       <c r="D100" t="s">
-        <v>132</v>
+        <v>356</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2646,7 +2811,7 @@
         <v>81</v>
       </c>
       <c r="D101" t="s">
-        <v>131</v>
+        <v>355</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2657,7 +2822,7 @@
         <v>80</v>
       </c>
       <c r="D102" t="s">
-        <v>130</v>
+        <v>354</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2668,7 +2833,7 @@
         <v>79</v>
       </c>
       <c r="D103" t="s">
-        <v>129</v>
+        <v>353</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2679,7 +2844,7 @@
         <v>78</v>
       </c>
       <c r="D104" t="s">
-        <v>70</v>
+        <v>351</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2690,7 +2855,7 @@
         <v>77</v>
       </c>
       <c r="D105" t="s">
-        <v>128</v>
+        <v>352</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2701,7 +2866,7 @@
         <v>76</v>
       </c>
       <c r="D106" t="s">
-        <v>70</v>
+        <v>351</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2712,7 +2877,7 @@
         <v>75</v>
       </c>
       <c r="D107" t="s">
-        <v>127</v>
+        <v>350</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2723,7 +2888,7 @@
         <v>74</v>
       </c>
       <c r="D108" t="s">
-        <v>126</v>
+        <v>349</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2734,7 +2899,7 @@
         <v>73</v>
       </c>
       <c r="D109" t="s">
-        <v>126</v>
+        <v>349</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2745,7 +2910,7 @@
         <v>72</v>
       </c>
       <c r="D110" t="s">
-        <v>125</v>
+        <v>348</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2756,7 +2921,7 @@
         <v>71</v>
       </c>
       <c r="D111" t="s">
-        <v>124</v>
+        <v>347</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2767,7 +2932,7 @@
         <v>70</v>
       </c>
       <c r="D112" t="s">
-        <v>123</v>
+        <v>346</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2778,7 +2943,7 @@
         <v>69</v>
       </c>
       <c r="D113" t="s">
-        <v>122</v>
+        <v>345</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2789,7 +2954,7 @@
         <v>68</v>
       </c>
       <c r="D114" t="s">
-        <v>121</v>
+        <v>344</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2800,7 +2965,7 @@
         <v>67</v>
       </c>
       <c r="D115" t="s">
-        <v>120</v>
+        <v>343</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2811,7 +2976,7 @@
         <v>66</v>
       </c>
       <c r="D116" t="s">
-        <v>119</v>
+        <v>342</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -2822,7 +2987,7 @@
         <v>65</v>
       </c>
       <c r="D117" t="s">
-        <v>303</v>
+        <v>341</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -2833,7 +2998,7 @@
         <v>64</v>
       </c>
       <c r="D118" t="s">
-        <v>117</v>
+        <v>340</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2844,7 +3009,7 @@
         <v>63</v>
       </c>
       <c r="D119" t="s">
-        <v>116</v>
+        <v>339</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -2855,7 +3020,7 @@
         <v>62</v>
       </c>
       <c r="D120" t="s">
-        <v>115</v>
+        <v>338</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -2866,7 +3031,7 @@
         <v>61</v>
       </c>
       <c r="D121" t="s">
-        <v>114</v>
+        <v>337</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2877,7 +3042,7 @@
         <v>60</v>
       </c>
       <c r="D122" t="s">
-        <v>113</v>
+        <v>336</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -2888,7 +3053,7 @@
         <v>59</v>
       </c>
       <c r="D123" t="s">
-        <v>112</v>
+        <v>335</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -2899,7 +3064,7 @@
         <v>58</v>
       </c>
       <c r="D124" t="s">
-        <v>111</v>
+        <v>334</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -2910,7 +3075,7 @@
         <v>57</v>
       </c>
       <c r="D125" t="s">
-        <v>110</v>
+        <v>333</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -2921,7 +3086,7 @@
         <v>56</v>
       </c>
       <c r="D126" t="s">
-        <v>109</v>
+        <v>332</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -2932,7 +3097,7 @@
         <v>55</v>
       </c>
       <c r="D127" t="s">
-        <v>301</v>
+        <v>331</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -2944,10 +3109,10 @@
       </c>
       <c r="C128" s="4"/>
       <c r="D128" t="s">
-        <v>299</v>
+        <v>329</v>
       </c>
       <c r="E128" t="s">
-        <v>300</v>
+        <v>330</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3261,7 +3426,7 @@
         <v>254</v>
       </c>
       <c r="E150" t="s">
-        <v>255</v>
+        <v>328</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -3397,7 +3562,7 @@
         <v>239</v>
       </c>
       <c r="E159" t="s">
-        <v>240</v>
+        <v>327</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -3408,7 +3573,7 @@
         <v>26</v>
       </c>
       <c r="D160" t="s">
-        <v>237</v>
+        <v>310</v>
       </c>
       <c r="E160" t="s">
         <v>238</v>
@@ -3422,7 +3587,7 @@
         <v>25</v>
       </c>
       <c r="D161" t="s">
-        <v>235</v>
+        <v>311</v>
       </c>
       <c r="E161" t="s">
         <v>236</v>
@@ -3453,7 +3618,7 @@
         <v>231</v>
       </c>
       <c r="E163" t="s">
-        <v>232</v>
+        <v>312</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -3481,7 +3646,7 @@
         <v>227</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>228</v>
@@ -3498,7 +3663,7 @@
         <v>226</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>228</v>
@@ -3515,9 +3680,11 @@
         <v>224</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F167" s="2"/>
+        <v>315</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="168" spans="1:6">
       <c r="A168">
@@ -3541,10 +3708,10 @@
         <v>17</v>
       </c>
       <c r="D169" t="s">
-        <v>220</v>
+        <v>317</v>
       </c>
       <c r="E169" t="s">
-        <v>221</v>
+        <v>318</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -3558,7 +3725,7 @@
         <v>218</v>
       </c>
       <c r="E170" t="s">
-        <v>219</v>
+        <v>319</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -3572,7 +3739,7 @@
         <v>216</v>
       </c>
       <c r="E171" t="s">
-        <v>217</v>
+        <v>320</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -3583,10 +3750,10 @@
         <v>14</v>
       </c>
       <c r="D172" t="s">
-        <v>214</v>
+        <v>322</v>
       </c>
       <c r="E172" t="s">
-        <v>215</v>
+        <v>321</v>
       </c>
     </row>
     <row r="173" spans="1:6">
@@ -3611,10 +3778,10 @@
         <v>12</v>
       </c>
       <c r="D174" t="s">
-        <v>210</v>
+        <v>323</v>
       </c>
       <c r="E174" t="s">
-        <v>211</v>
+        <v>324</v>
       </c>
     </row>
     <row r="175" spans="1:6">
@@ -3656,7 +3823,7 @@
         <v>204</v>
       </c>
       <c r="E177" t="s">
-        <v>205</v>
+        <v>325</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -3670,7 +3837,7 @@
         <v>202</v>
       </c>
       <c r="E178" t="s">
-        <v>203</v>
+        <v>326</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -3681,10 +3848,10 @@
         <v>7</v>
       </c>
       <c r="D179" t="s">
-        <v>200</v>
+        <v>309</v>
       </c>
       <c r="E179" t="s">
-        <v>201</v>
+        <v>308</v>
       </c>
     </row>
     <row r="180" spans="1:6">
@@ -3768,10 +3935,10 @@
         <v>1</v>
       </c>
       <c r="D185" t="s">
-        <v>187</v>
+        <v>362</v>
       </c>
       <c r="E185" t="s">
-        <v>188</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>